<commit_message>
Fix priors and parameters for stage distribution
</commit_message>
<xml_diff>
--- a/_ground_truth/constant_priors.xlsx
+++ b/_ground_truth/constant_priors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/Repositories/tutorial_cancer_modeling_des/_ground_truth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC7D7EF-B5B4-8F49-BFF2-BB51BA0B76B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE517F9-BABA-5340-9EFA-67D575EC97A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1080" windowWidth="27640" windowHeight="16940" xr2:uid="{2C803228-1F19-7743-A522-FA2F126D8935}"/>
   </bookViews>
@@ -436,7 +436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3150F6F3-3F07-174B-9F21-1FF8B839C0EF}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -559,10 +561,10 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>-0.01</v>
+        <v>-0.05</v>
       </c>
       <c r="F6">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -580,10 +582,10 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>-2.5000000000000001E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="F7">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -601,10 +603,10 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="F8">
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>